<commit_message>
Update testing logs 2021-04-10
</commit_message>
<xml_diff>
--- a/PEARL_MOOS_testing_notes.xlsx
+++ b/PEARL_MOOS_testing_notes.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/maha/pearl_testing_logs/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{481C3B34-1899-A04B-835B-7C2D8C28F1C8}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{32A65013-436D-9943-907B-2946882E169C}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="460" windowWidth="24420" windowHeight="15540" xr2:uid="{CE7898E4-CB96-184C-9C00-2CBDA86B470B}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="619" uniqueCount="353">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="641" uniqueCount="365">
   <si>
     <t>Date</t>
   </si>
@@ -1368,12 +1368,52 @@
   <si>
     <t>LOG_PEARL_SQUARE_6_4_2021_____15_17_20</t>
   </si>
+  <si>
+    <t>Suntracking Deadband</t>
+  </si>
+  <si>
+    <t>- PEARL anchored, with lots of slack, +/- 0 deg deadband (aka "best case scenario" where only needs thrust to maintain heading, no movement from stationkeep circle, and as close as possible to max power generation at 0 deg deadband)
+- 20 min test</t>
+  </si>
+  <si>
+    <t>- rerun above with suntracking OFF
+- 20 min test</t>
+  </si>
+  <si>
+    <t xml:space="preserve">- PEARL anchored, with lots of slack, +/- 0 deg deadband (aka "best case scenario" where only needs thrust to maintain heading, no movement from stationkeep circle, and as close as possible to max power generation at 0 deg deadband)
+- 20 min test
+- clouds rolled in </t>
+  </si>
+  <si>
+    <t>- only conducted one star and one perimeter for 20min mission used to collect drone footage</t>
+  </si>
+  <si>
+    <t>LOG_PEARL_SIMPLE_10_4_2021_____14_36_51</t>
+  </si>
+  <si>
+    <t>LOG_PEARL_SIMPLE_10_4_2021_____14_58_01</t>
+  </si>
+  <si>
+    <t>LOG_PEARL_SIMPLE_10_4_2021_____15_19_23</t>
+  </si>
+  <si>
+    <t>LOG_PEARL_SIMPLE_10_4_2021_____15_40_42</t>
+  </si>
+  <si>
+    <t>LOG_PEARL_SIMPLE_10_4_2021_____16_02_27</t>
+  </si>
+  <si>
+    <t>LOG_PEARL_SIMPLE_10_4_2021_____16_23_34</t>
+  </si>
+  <si>
+    <t>LOG_PEARL_SQUARE_10_4_2021_____17_15_46</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -1402,15 +1442,8 @@
       <name val="Helvetica"/>
       <family val="2"/>
     </font>
-    <font>
-      <sz val="12"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
   </fonts>
-  <fills count="9">
+  <fills count="10">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -1459,6 +1492,12 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0" tint="-0.14999847407452621"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="1">
     <border>
@@ -1472,7 +1511,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="58">
+  <cellXfs count="63">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -1551,6 +1590,13 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="9" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="18" fontId="0" fillId="9" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" quotePrefix="1" applyFill="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
   </cellXfs>
@@ -1872,28 +1918,28 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6C322D9A-DAA8-F94B-8299-5D36BBA36BB2}">
-  <dimension ref="A1:L158"/>
+  <dimension ref="A1:M165"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A151" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D161" sqref="D161"/>
+      <pane ySplit="1" topLeftCell="A157" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="D165" sqref="D165"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="2" max="2" width="16.5" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="35.1640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="43.6640625" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="55.83203125" customWidth="1"/>
     <col min="5" max="5" width="7.83203125" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="7.33203125" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="7.83203125" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="9.33203125" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="8.83203125" bestFit="1" customWidth="1"/>
-    <col min="10" max="11" width="8.83203125" customWidth="1"/>
-    <col min="12" max="12" width="80.1640625" customWidth="1"/>
+    <col min="10" max="12" width="8.83203125" customWidth="1"/>
+    <col min="13" max="13" width="80.1640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1925,13 +1971,16 @@
         <v>41</v>
       </c>
       <c r="K1" s="1" t="s">
+        <v>353</v>
+      </c>
+      <c r="L1" s="1" t="s">
         <v>115</v>
       </c>
-      <c r="L1" s="1" t="s">
+      <c r="M1" s="1" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:12" ht="34" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:13" ht="34" x14ac:dyDescent="0.2">
       <c r="A2" s="5">
         <v>44277</v>
       </c>
@@ -1962,11 +2011,11 @@
       <c r="J2">
         <v>0.3</v>
       </c>
-      <c r="L2" s="2" t="s">
+      <c r="M2" s="2" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A3" s="5">
         <v>44277</v>
       </c>
@@ -1997,11 +2046,11 @@
       <c r="J3">
         <v>0.3</v>
       </c>
-      <c r="L3" t="s">
+      <c r="M3" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="4" spans="1:12" ht="85" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:13" ht="85" x14ac:dyDescent="0.2">
       <c r="A4" s="5">
         <v>44277</v>
       </c>
@@ -2032,11 +2081,11 @@
       <c r="J4">
         <v>0.3</v>
       </c>
-      <c r="L4" s="2" t="s">
+      <c r="M4" s="2" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="5" spans="1:12" ht="68" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:13" ht="68" x14ac:dyDescent="0.2">
       <c r="A5" s="5">
         <v>44277</v>
       </c>
@@ -2067,11 +2116,11 @@
       <c r="J5">
         <v>0.3</v>
       </c>
-      <c r="L5" s="2" t="s">
+      <c r="M5" s="2" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="6" spans="1:12" ht="272" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:13" ht="272" x14ac:dyDescent="0.2">
       <c r="A6" s="5">
         <v>44277</v>
       </c>
@@ -2087,11 +2136,11 @@
       <c r="J6">
         <v>0.3</v>
       </c>
-      <c r="L6" s="4" t="s">
+      <c r="M6" s="4" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="7" spans="1:12" ht="102" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:13" ht="102" x14ac:dyDescent="0.2">
       <c r="A7" s="5">
         <v>44277</v>
       </c>
@@ -2122,11 +2171,11 @@
       <c r="J7">
         <v>0.3</v>
       </c>
-      <c r="L7" s="4" t="s">
+      <c r="M7" s="4" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="8" spans="1:12" ht="34" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:13" ht="34" x14ac:dyDescent="0.2">
       <c r="A8" s="5">
         <v>44277</v>
       </c>
@@ -2157,11 +2206,11 @@
       <c r="J8">
         <v>0.3</v>
       </c>
-      <c r="L8" s="4" t="s">
+      <c r="M8" s="4" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="9" spans="1:12" ht="136" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:13" ht="136" x14ac:dyDescent="0.2">
       <c r="A9" s="5">
         <v>44277</v>
       </c>
@@ -2192,11 +2241,11 @@
       <c r="J9">
         <v>0.3</v>
       </c>
-      <c r="L9" s="4" t="s">
+      <c r="M9" s="4" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="10" spans="1:12" ht="51" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:13" ht="51" x14ac:dyDescent="0.2">
       <c r="A10" s="5">
         <v>44277</v>
       </c>
@@ -2227,11 +2276,11 @@
       <c r="J10">
         <v>0.3</v>
       </c>
-      <c r="L10" s="2" t="s">
+      <c r="M10" s="2" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="11" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A11" s="5">
         <v>44278</v>
       </c>
@@ -2262,11 +2311,11 @@
       <c r="J11">
         <v>0.3</v>
       </c>
-      <c r="L11" t="s">
+      <c r="M11" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="12" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A12" s="5">
         <v>44278</v>
       </c>
@@ -2297,11 +2346,11 @@
       <c r="J12">
         <v>0.3</v>
       </c>
-      <c r="L12" t="s">
+      <c r="M12" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="13" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A13" s="5">
         <v>44278</v>
       </c>
@@ -2332,11 +2381,11 @@
       <c r="J13">
         <v>0.3</v>
       </c>
-      <c r="L13" t="s">
+      <c r="M13" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="14" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A14" s="5">
         <v>44278</v>
       </c>
@@ -2367,11 +2416,11 @@
       <c r="J14">
         <v>0.3</v>
       </c>
-      <c r="L14" t="s">
+      <c r="M14" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="15" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A15" s="5">
         <v>44278</v>
       </c>
@@ -2402,11 +2451,11 @@
       <c r="J15">
         <v>0.3</v>
       </c>
-      <c r="L15" t="s">
+      <c r="M15" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="16" spans="1:12" ht="34" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:13" ht="34" x14ac:dyDescent="0.2">
       <c r="A16" s="5">
         <v>44278</v>
       </c>
@@ -2437,11 +2486,11 @@
       <c r="J16">
         <v>0.3</v>
       </c>
-      <c r="L16" s="2" t="s">
+      <c r="M16" s="2" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="17" spans="1:12" ht="85" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:13" ht="85" x14ac:dyDescent="0.2">
       <c r="A17" s="5">
         <v>44278</v>
       </c>
@@ -2472,11 +2521,11 @@
       <c r="J17">
         <v>0.3</v>
       </c>
-      <c r="L17" s="2" t="s">
+      <c r="M17" s="2" t="s">
         <v>65</v>
       </c>
     </row>
-    <row r="18" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A18" s="5">
         <v>44278</v>
       </c>
@@ -2507,11 +2556,11 @@
       <c r="J18">
         <v>0.3</v>
       </c>
-      <c r="L18" t="s">
+      <c r="M18" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="19" spans="1:12" ht="17" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:13" ht="17" x14ac:dyDescent="0.2">
       <c r="A19" s="5">
         <v>44278</v>
       </c>
@@ -2542,11 +2591,11 @@
       <c r="J19">
         <v>0.3</v>
       </c>
-      <c r="L19" s="2" t="s">
+      <c r="M19" s="2" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="20" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A20" s="5">
         <v>44278</v>
       </c>
@@ -2577,11 +2626,11 @@
       <c r="J20">
         <v>0.3</v>
       </c>
-      <c r="L20" t="s">
+      <c r="M20" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="21" spans="1:12" ht="66" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:13" ht="66" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A21" s="5">
         <v>44278</v>
       </c>
@@ -2612,11 +2661,11 @@
       <c r="J21">
         <v>0.5</v>
       </c>
-      <c r="L21" s="4" t="s">
+      <c r="M21" s="4" t="s">
         <v>42</v>
       </c>
     </row>
-    <row r="22" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A22" s="5">
         <v>44278</v>
       </c>
@@ -2647,11 +2696,11 @@
       <c r="J22">
         <v>0.5</v>
       </c>
-      <c r="L22" s="6" t="s">
+      <c r="M22" s="6" t="s">
         <v>43</v>
       </c>
     </row>
-    <row r="23" spans="1:12" ht="51" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:13" ht="51" x14ac:dyDescent="0.2">
       <c r="A23" s="5">
         <v>44278</v>
       </c>
@@ -2682,11 +2731,11 @@
       <c r="J23">
         <v>0.5</v>
       </c>
-      <c r="L23" s="4" t="s">
+      <c r="M23" s="4" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="24" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A24" s="5">
         <v>44278</v>
       </c>
@@ -2717,11 +2766,11 @@
       <c r="J24">
         <v>0.5</v>
       </c>
-      <c r="L24" s="6" t="s">
+      <c r="M24" s="6" t="s">
         <v>45</v>
       </c>
     </row>
-    <row r="25" spans="1:12" ht="34" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:13" ht="34" x14ac:dyDescent="0.2">
       <c r="A25" s="5">
         <v>44278</v>
       </c>
@@ -2752,11 +2801,11 @@
       <c r="J25">
         <v>0.5</v>
       </c>
-      <c r="L25" s="4" t="s">
+      <c r="M25" s="4" t="s">
         <v>46</v>
       </c>
     </row>
-    <row r="26" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A26" s="5">
         <v>44278</v>
       </c>
@@ -2787,11 +2836,11 @@
       <c r="J26">
         <v>0.5</v>
       </c>
-      <c r="L26" s="6" t="s">
+      <c r="M26" s="6" t="s">
         <v>47</v>
       </c>
     </row>
-    <row r="27" spans="1:12" ht="17" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:13" ht="17" x14ac:dyDescent="0.2">
       <c r="A27" s="5">
         <v>44278</v>
       </c>
@@ -2822,11 +2871,11 @@
       <c r="J27">
         <v>0.5</v>
       </c>
-      <c r="L27" s="4" t="s">
+      <c r="M27" s="4" t="s">
         <v>48</v>
       </c>
     </row>
-    <row r="28" spans="1:12" ht="34" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:13" ht="34" x14ac:dyDescent="0.2">
       <c r="A28" s="5">
         <v>44278</v>
       </c>
@@ -2857,11 +2906,11 @@
       <c r="J28">
         <v>0.5</v>
       </c>
-      <c r="L28" s="4" t="s">
+      <c r="M28" s="4" t="s">
         <v>49</v>
       </c>
     </row>
-    <row r="29" spans="1:12" ht="34" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:13" ht="34" x14ac:dyDescent="0.2">
       <c r="A29" s="5">
         <v>44278</v>
       </c>
@@ -2892,11 +2941,11 @@
       <c r="J29">
         <v>0.5</v>
       </c>
-      <c r="L29" s="4" t="s">
+      <c r="M29" s="4" t="s">
         <v>50</v>
       </c>
     </row>
-    <row r="30" spans="1:12" ht="34" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:13" ht="34" x14ac:dyDescent="0.2">
       <c r="A30" s="5">
         <v>44278</v>
       </c>
@@ -2927,11 +2976,11 @@
       <c r="J30">
         <v>0.5</v>
       </c>
-      <c r="L30" s="4" t="s">
+      <c r="M30" s="4" t="s">
         <v>51</v>
       </c>
     </row>
-    <row r="31" spans="1:12" ht="17" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:13" ht="17" x14ac:dyDescent="0.2">
       <c r="A31" s="5">
         <v>44278</v>
       </c>
@@ -2962,11 +3011,11 @@
       <c r="J31">
         <v>0.5</v>
       </c>
-      <c r="L31" s="4" t="s">
+      <c r="M31" s="4" t="s">
         <v>52</v>
       </c>
     </row>
-    <row r="32" spans="1:12" ht="51" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:13" ht="51" x14ac:dyDescent="0.2">
       <c r="A32" s="5">
         <v>44278</v>
       </c>
@@ -2997,11 +3046,11 @@
       <c r="J32">
         <v>0.5</v>
       </c>
-      <c r="L32" s="4" t="s">
+      <c r="M32" s="4" t="s">
         <v>53</v>
       </c>
     </row>
-    <row r="33" spans="1:12" ht="17" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:13" ht="17" x14ac:dyDescent="0.2">
       <c r="A33" s="5">
         <v>44278</v>
       </c>
@@ -3032,11 +3081,11 @@
       <c r="J33">
         <v>0.5</v>
       </c>
-      <c r="L33" s="4" t="s">
+      <c r="M33" s="4" t="s">
         <v>54</v>
       </c>
     </row>
-    <row r="34" spans="1:12" ht="17" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:13" ht="17" x14ac:dyDescent="0.2">
       <c r="A34" s="5">
         <v>44278</v>
       </c>
@@ -3067,11 +3116,11 @@
       <c r="J34">
         <v>0.5</v>
       </c>
-      <c r="L34" s="4" t="s">
+      <c r="M34" s="4" t="s">
         <v>55</v>
       </c>
     </row>
-    <row r="35" spans="1:12" ht="34" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:13" ht="34" x14ac:dyDescent="0.2">
       <c r="A35" s="5">
         <v>44278</v>
       </c>
@@ -3102,11 +3151,11 @@
       <c r="J35">
         <v>0.5</v>
       </c>
-      <c r="L35" s="4" t="s">
+      <c r="M35" s="4" t="s">
         <v>56</v>
       </c>
     </row>
-    <row r="36" spans="1:12" ht="17" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:13" ht="17" x14ac:dyDescent="0.2">
       <c r="A36" s="5">
         <v>44279</v>
       </c>
@@ -3137,11 +3186,11 @@
       <c r="J36">
         <v>0.5</v>
       </c>
-      <c r="L36" s="4" t="s">
+      <c r="M36" s="4" t="s">
         <v>84</v>
       </c>
     </row>
-    <row r="37" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A37" s="5">
         <v>44279</v>
       </c>
@@ -3172,11 +3221,11 @@
       <c r="J37">
         <v>0.5</v>
       </c>
-      <c r="L37" s="6" t="s">
+      <c r="M37" s="6" t="s">
         <v>85</v>
       </c>
     </row>
-    <row r="38" spans="1:12" s="36" customFormat="1" ht="34" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:13" s="36" customFormat="1" ht="34" x14ac:dyDescent="0.2">
       <c r="A38" s="41">
         <v>44279</v>
       </c>
@@ -3207,14 +3256,14 @@
       <c r="J38" s="36">
         <v>0.5</v>
       </c>
-      <c r="K38" s="36" t="s">
+      <c r="L38" s="36" t="s">
         <v>117</v>
       </c>
-      <c r="L38" s="37" t="s">
+      <c r="M38" s="37" t="s">
         <v>250</v>
       </c>
     </row>
-    <row r="39" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A39" s="5">
         <v>44279</v>
       </c>
@@ -3245,14 +3294,14 @@
       <c r="J39">
         <v>0.5</v>
       </c>
-      <c r="K39" t="s">
+      <c r="L39" t="s">
         <v>117</v>
       </c>
-      <c r="L39" s="6" t="s">
+      <c r="M39" s="6" t="s">
         <v>86</v>
       </c>
     </row>
-    <row r="40" spans="1:12" s="20" customFormat="1" ht="17" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:13" s="20" customFormat="1" ht="17" x14ac:dyDescent="0.2">
       <c r="A40" s="18">
         <v>44279</v>
       </c>
@@ -3283,14 +3332,14 @@
       <c r="J40" s="20">
         <v>0.5</v>
       </c>
-      <c r="K40" s="20" t="s">
+      <c r="L40" s="20" t="s">
         <v>116</v>
       </c>
-      <c r="L40" s="21" t="s">
+      <c r="M40" s="21" t="s">
         <v>87</v>
       </c>
     </row>
-    <row r="41" spans="1:12" ht="17" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:13" ht="17" x14ac:dyDescent="0.2">
       <c r="A41" s="5">
         <v>44279</v>
       </c>
@@ -3321,14 +3370,14 @@
       <c r="J41">
         <v>0.5</v>
       </c>
-      <c r="K41" t="s">
+      <c r="L41" t="s">
         <v>117</v>
       </c>
-      <c r="L41" s="4" t="s">
+      <c r="M41" s="4" t="s">
         <v>88</v>
       </c>
     </row>
-    <row r="42" spans="1:12" s="36" customFormat="1" ht="102" x14ac:dyDescent="0.2">
+    <row r="42" spans="1:13" s="36" customFormat="1" ht="102" x14ac:dyDescent="0.2">
       <c r="A42" s="33">
         <v>44279</v>
       </c>
@@ -3359,14 +3408,15 @@
       <c r="J42" s="35">
         <v>0.5</v>
       </c>
-      <c r="K42" s="35" t="s">
+      <c r="K42" s="35"/>
+      <c r="L42" s="35" t="s">
         <v>122</v>
       </c>
-      <c r="L42" s="48" t="s">
+      <c r="M42" s="48" t="s">
         <v>208</v>
       </c>
     </row>
-    <row r="43" spans="1:12" ht="17" x14ac:dyDescent="0.2">
+    <row r="43" spans="1:13" ht="17" x14ac:dyDescent="0.2">
       <c r="A43" s="7">
         <v>44279</v>
       </c>
@@ -3397,14 +3447,15 @@
       <c r="J43" s="9">
         <v>0.5</v>
       </c>
-      <c r="K43" s="9" t="s">
+      <c r="K43" s="9"/>
+      <c r="L43" s="9" t="s">
         <v>117</v>
       </c>
-      <c r="L43" s="4" t="s">
+      <c r="M43" s="4" t="s">
         <v>89</v>
       </c>
     </row>
-    <row r="44" spans="1:12" s="11" customFormat="1" ht="17" x14ac:dyDescent="0.2">
+    <row r="44" spans="1:13" s="11" customFormat="1" ht="17" x14ac:dyDescent="0.2">
       <c r="A44" s="13">
         <v>44279</v>
       </c>
@@ -3435,14 +3486,15 @@
       <c r="J44" s="14">
         <v>0.5</v>
       </c>
-      <c r="K44" s="14" t="s">
+      <c r="K44" s="14"/>
+      <c r="L44" s="14" t="s">
         <v>116</v>
       </c>
-      <c r="L44" s="12" t="s">
+      <c r="M44" s="12" t="s">
         <v>90</v>
       </c>
     </row>
-    <row r="45" spans="1:12" ht="34" x14ac:dyDescent="0.2">
+    <row r="45" spans="1:13" ht="34" x14ac:dyDescent="0.2">
       <c r="A45" s="7">
         <v>44280</v>
       </c>
@@ -3473,14 +3525,15 @@
       <c r="J45" s="9">
         <v>0.5</v>
       </c>
-      <c r="K45" s="9" t="s">
+      <c r="K45" s="9"/>
+      <c r="L45" s="9" t="s">
         <v>117</v>
       </c>
-      <c r="L45" s="4" t="s">
+      <c r="M45" s="4" t="s">
         <v>101</v>
       </c>
     </row>
-    <row r="46" spans="1:12" s="36" customFormat="1" ht="34" x14ac:dyDescent="0.2">
+    <row r="46" spans="1:13" s="36" customFormat="1" ht="34" x14ac:dyDescent="0.2">
       <c r="A46" s="33">
         <v>44280</v>
       </c>
@@ -3511,14 +3564,15 @@
       <c r="J46" s="35">
         <v>0.5</v>
       </c>
-      <c r="K46" s="35" t="s">
+      <c r="K46" s="35"/>
+      <c r="L46" s="35" t="s">
         <v>117</v>
       </c>
-      <c r="L46" s="37" t="s">
+      <c r="M46" s="37" t="s">
         <v>251</v>
       </c>
     </row>
-    <row r="47" spans="1:12" ht="17" x14ac:dyDescent="0.2">
+    <row r="47" spans="1:13" ht="17" x14ac:dyDescent="0.2">
       <c r="A47" s="7">
         <v>44280</v>
       </c>
@@ -3549,14 +3603,15 @@
       <c r="J47" s="9">
         <v>0.5</v>
       </c>
-      <c r="K47" s="9" t="s">
+      <c r="K47" s="9"/>
+      <c r="L47" s="9" t="s">
         <v>117</v>
       </c>
-      <c r="L47" s="2" t="s">
+      <c r="M47" s="2" t="s">
         <v>102</v>
       </c>
     </row>
-    <row r="48" spans="1:12" s="36" customFormat="1" ht="68" x14ac:dyDescent="0.2">
+    <row r="48" spans="1:13" s="36" customFormat="1" ht="68" x14ac:dyDescent="0.2">
       <c r="A48" s="33">
         <v>44280</v>
       </c>
@@ -3587,14 +3642,15 @@
       <c r="J48" s="35">
         <v>0.5</v>
       </c>
-      <c r="K48" s="35" t="s">
+      <c r="K48" s="35"/>
+      <c r="L48" s="35" t="s">
         <v>117</v>
       </c>
-      <c r="L48" s="37" t="s">
+      <c r="M48" s="37" t="s">
         <v>252</v>
       </c>
     </row>
-    <row r="49" spans="1:12" s="24" customFormat="1" ht="17" x14ac:dyDescent="0.2">
+    <row r="49" spans="1:13" s="24" customFormat="1" ht="17" x14ac:dyDescent="0.2">
       <c r="A49" s="22">
         <v>44280</v>
       </c>
@@ -3625,14 +3681,15 @@
       <c r="J49" s="23">
         <v>0.5</v>
       </c>
-      <c r="K49" s="23" t="s">
+      <c r="K49" s="23"/>
+      <c r="L49" s="23" t="s">
         <v>116</v>
       </c>
-      <c r="L49" s="26" t="s">
+      <c r="M49" s="26" t="s">
         <v>103</v>
       </c>
     </row>
-    <row r="50" spans="1:12" ht="34" x14ac:dyDescent="0.2">
+    <row r="50" spans="1:13" ht="34" x14ac:dyDescent="0.2">
       <c r="A50" s="7">
         <v>44280</v>
       </c>
@@ -3663,14 +3720,15 @@
       <c r="J50" s="9">
         <v>0.5</v>
       </c>
-      <c r="K50" s="9" t="s">
+      <c r="K50" s="9"/>
+      <c r="L50" s="9" t="s">
         <v>117</v>
       </c>
-      <c r="L50" s="4" t="s">
+      <c r="M50" s="4" t="s">
         <v>105</v>
       </c>
     </row>
-    <row r="51" spans="1:12" s="24" customFormat="1" ht="17" x14ac:dyDescent="0.2">
+    <row r="51" spans="1:13" s="24" customFormat="1" ht="17" x14ac:dyDescent="0.2">
       <c r="A51" s="22">
         <v>44280</v>
       </c>
@@ -3701,14 +3759,15 @@
       <c r="J51" s="23">
         <v>0.5</v>
       </c>
-      <c r="K51" s="23" t="s">
+      <c r="K51" s="23"/>
+      <c r="L51" s="23" t="s">
         <v>116</v>
       </c>
-      <c r="L51" s="26" t="s">
+      <c r="M51" s="26" t="s">
         <v>104</v>
       </c>
     </row>
-    <row r="52" spans="1:12" ht="17" x14ac:dyDescent="0.2">
+    <row r="52" spans="1:13" ht="17" x14ac:dyDescent="0.2">
       <c r="A52" s="5">
         <v>44280</v>
       </c>
@@ -3739,14 +3798,15 @@
       <c r="J52" s="9">
         <v>0.5</v>
       </c>
-      <c r="K52" s="9" t="s">
+      <c r="K52" s="9"/>
+      <c r="L52" s="9" t="s">
         <v>117</v>
       </c>
-      <c r="L52" s="4" t="s">
+      <c r="M52" s="4" t="s">
         <v>106</v>
       </c>
     </row>
-    <row r="53" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="53" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A53" s="5">
         <v>44282</v>
       </c>
@@ -3777,14 +3837,14 @@
       <c r="J53">
         <v>0.5</v>
       </c>
-      <c r="K53" t="s">
+      <c r="L53" t="s">
         <v>117</v>
       </c>
-      <c r="L53" s="6" t="s">
+      <c r="M53" s="6" t="s">
         <v>118</v>
       </c>
     </row>
-    <row r="54" spans="1:12" s="20" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="54" spans="1:13" s="20" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A54" s="18">
         <v>44282</v>
       </c>
@@ -3815,11 +3875,11 @@
       <c r="J54" s="20">
         <v>0.5</v>
       </c>
-      <c r="K54" s="20" t="s">
+      <c r="L54" s="20" t="s">
         <v>116</v>
       </c>
     </row>
-    <row r="55" spans="1:12" ht="34" x14ac:dyDescent="0.2">
+    <row r="55" spans="1:13" ht="34" x14ac:dyDescent="0.2">
       <c r="A55" s="5">
         <v>44282</v>
       </c>
@@ -3850,14 +3910,14 @@
       <c r="J55">
         <v>0.5</v>
       </c>
-      <c r="K55" t="s">
+      <c r="L55" t="s">
         <v>122</v>
       </c>
-      <c r="L55" s="4" t="s">
+      <c r="M55" s="4" t="s">
         <v>119</v>
       </c>
     </row>
-    <row r="56" spans="1:12" ht="68" x14ac:dyDescent="0.2">
+    <row r="56" spans="1:13" ht="68" x14ac:dyDescent="0.2">
       <c r="A56" s="5">
         <v>44282</v>
       </c>
@@ -3888,14 +3948,14 @@
       <c r="J56">
         <v>0.5</v>
       </c>
-      <c r="K56" t="s">
+      <c r="L56" t="s">
         <v>122</v>
       </c>
-      <c r="L56" s="4" t="s">
+      <c r="M56" s="4" t="s">
         <v>120</v>
       </c>
     </row>
-    <row r="57" spans="1:12" ht="17" x14ac:dyDescent="0.2">
+    <row r="57" spans="1:13" ht="17" x14ac:dyDescent="0.2">
       <c r="A57" s="5">
         <v>44282</v>
       </c>
@@ -3926,14 +3986,14 @@
       <c r="J57">
         <v>0.5</v>
       </c>
-      <c r="K57" t="s">
+      <c r="L57" t="s">
         <v>122</v>
       </c>
-      <c r="L57" s="4" t="s">
+      <c r="M57" s="4" t="s">
         <v>121</v>
       </c>
     </row>
-    <row r="58" spans="1:12" s="36" customFormat="1" ht="17" x14ac:dyDescent="0.2">
+    <row r="58" spans="1:13" s="36" customFormat="1" ht="17" x14ac:dyDescent="0.2">
       <c r="A58" s="41">
         <v>44282</v>
       </c>
@@ -3964,14 +4024,14 @@
       <c r="J58" s="36">
         <v>0.5</v>
       </c>
-      <c r="K58" s="36" t="s">
+      <c r="L58" s="36" t="s">
         <v>117</v>
       </c>
-      <c r="L58" s="37" t="s">
+      <c r="M58" s="37" t="s">
         <v>249</v>
       </c>
     </row>
-    <row r="59" spans="1:12" s="20" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="59" spans="1:13" s="20" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A59" s="18">
         <v>44282</v>
       </c>
@@ -4002,11 +4062,11 @@
       <c r="J59" s="20">
         <v>0.5</v>
       </c>
-      <c r="K59" s="20" t="s">
+      <c r="L59" s="20" t="s">
         <v>116</v>
       </c>
     </row>
-    <row r="60" spans="1:12" s="20" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="60" spans="1:13" s="20" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A60" s="18">
         <v>44282</v>
       </c>
@@ -4037,11 +4097,11 @@
       <c r="J60" s="20">
         <v>0.5</v>
       </c>
-      <c r="K60" s="20" t="s">
+      <c r="L60" s="20" t="s">
         <v>116</v>
       </c>
     </row>
-    <row r="61" spans="1:12" s="20" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="61" spans="1:13" s="20" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A61" s="18">
         <v>44282</v>
       </c>
@@ -4072,11 +4132,11 @@
       <c r="J61" s="20">
         <v>0.5</v>
       </c>
-      <c r="K61" s="20" t="s">
+      <c r="L61" s="20" t="s">
         <v>116</v>
       </c>
     </row>
-    <row r="62" spans="1:12" s="31" customFormat="1" ht="85" x14ac:dyDescent="0.2">
+    <row r="62" spans="1:13" s="31" customFormat="1" ht="85" x14ac:dyDescent="0.2">
       <c r="A62" s="29">
         <v>44282</v>
       </c>
@@ -4107,14 +4167,14 @@
       <c r="J62" s="31">
         <v>0.5</v>
       </c>
-      <c r="K62" s="31" t="s">
+      <c r="L62" s="31" t="s">
         <v>116</v>
       </c>
-      <c r="L62" s="32" t="s">
+      <c r="M62" s="32" t="s">
         <v>124</v>
       </c>
     </row>
-    <row r="63" spans="1:12" ht="68" x14ac:dyDescent="0.2">
+    <row r="63" spans="1:13" ht="68" x14ac:dyDescent="0.2">
       <c r="A63" s="5">
         <v>44282</v>
       </c>
@@ -4145,11 +4205,11 @@
       <c r="J63">
         <v>0.5</v>
       </c>
-      <c r="L63" s="4" t="s">
+      <c r="M63" s="4" t="s">
         <v>125</v>
       </c>
     </row>
-    <row r="64" spans="1:12" ht="51" x14ac:dyDescent="0.2">
+    <row r="64" spans="1:13" ht="51" x14ac:dyDescent="0.2">
       <c r="A64" s="5">
         <v>44282</v>
       </c>
@@ -4180,11 +4240,11 @@
       <c r="J64">
         <v>0.5</v>
       </c>
-      <c r="L64" s="4" t="s">
+      <c r="M64" s="4" t="s">
         <v>126</v>
       </c>
     </row>
-    <row r="65" spans="1:12" s="31" customFormat="1" ht="85" x14ac:dyDescent="0.2">
+    <row r="65" spans="1:13" s="31" customFormat="1" ht="85" x14ac:dyDescent="0.2">
       <c r="A65" s="29">
         <v>44282</v>
       </c>
@@ -4215,14 +4275,14 @@
       <c r="J65" s="31">
         <v>0.5</v>
       </c>
-      <c r="K65" s="31" t="s">
+      <c r="L65" s="31" t="s">
         <v>116</v>
       </c>
-      <c r="L65" s="32" t="s">
+      <c r="M65" s="32" t="s">
         <v>127</v>
       </c>
     </row>
-    <row r="66" spans="1:12" s="36" customFormat="1" ht="17" x14ac:dyDescent="0.2">
+    <row r="66" spans="1:13" s="36" customFormat="1" ht="17" x14ac:dyDescent="0.2">
       <c r="A66" s="33">
         <v>44280</v>
       </c>
@@ -4253,14 +4313,15 @@
       <c r="J66" s="35">
         <v>0.5</v>
       </c>
-      <c r="K66" s="35" t="s">
+      <c r="K66" s="35"/>
+      <c r="L66" s="35" t="s">
         <v>117</v>
       </c>
-      <c r="L66" s="37" t="s">
+      <c r="M66" s="37" t="s">
         <v>128</v>
       </c>
     </row>
-    <row r="67" spans="1:12" s="36" customFormat="1" ht="34" x14ac:dyDescent="0.2">
+    <row r="67" spans="1:13" s="36" customFormat="1" ht="34" x14ac:dyDescent="0.2">
       <c r="A67" s="33">
         <v>44280</v>
       </c>
@@ -4291,14 +4352,15 @@
       <c r="J67" s="35">
         <v>0.5</v>
       </c>
-      <c r="K67" s="35" t="s">
+      <c r="K67" s="35"/>
+      <c r="L67" s="35" t="s">
         <v>117</v>
       </c>
-      <c r="L67" s="37" t="s">
+      <c r="M67" s="37" t="s">
         <v>129</v>
       </c>
     </row>
-    <row r="68" spans="1:12" s="36" customFormat="1" ht="34" x14ac:dyDescent="0.2">
+    <row r="68" spans="1:13" s="36" customFormat="1" ht="34" x14ac:dyDescent="0.2">
       <c r="A68" s="33">
         <v>44280</v>
       </c>
@@ -4329,14 +4391,15 @@
       <c r="J68" s="35">
         <v>0.5</v>
       </c>
-      <c r="K68" s="35" t="s">
+      <c r="K68" s="35"/>
+      <c r="L68" s="35" t="s">
         <v>122</v>
       </c>
-      <c r="L68" s="37" t="s">
+      <c r="M68" s="37" t="s">
         <v>209</v>
       </c>
     </row>
-    <row r="69" spans="1:12" s="24" customFormat="1" ht="17" x14ac:dyDescent="0.2">
+    <row r="69" spans="1:13" s="24" customFormat="1" ht="17" x14ac:dyDescent="0.2">
       <c r="A69" s="22">
         <v>44280</v>
       </c>
@@ -4367,14 +4430,15 @@
       <c r="J69" s="23">
         <v>0.5</v>
       </c>
-      <c r="K69" s="23" t="s">
+      <c r="K69" s="23"/>
+      <c r="L69" s="23" t="s">
         <v>116</v>
       </c>
-      <c r="L69" s="26" t="s">
+      <c r="M69" s="26" t="s">
         <v>130</v>
       </c>
     </row>
-    <row r="70" spans="1:12" s="24" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="70" spans="1:13" s="24" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A70" s="22">
         <v>44280</v>
       </c>
@@ -4405,14 +4469,15 @@
       <c r="J70" s="23">
         <v>0.5</v>
       </c>
-      <c r="K70" s="23" t="s">
+      <c r="K70" s="23"/>
+      <c r="L70" s="23" t="s">
         <v>116</v>
       </c>
-      <c r="L70" s="38" t="s">
+      <c r="M70" s="38" t="s">
         <v>131</v>
       </c>
     </row>
-    <row r="71" spans="1:12" ht="17" x14ac:dyDescent="0.2">
+    <row r="71" spans="1:13" ht="17" x14ac:dyDescent="0.2">
       <c r="A71" s="5">
         <v>44280</v>
       </c>
@@ -4443,14 +4508,15 @@
       <c r="J71" s="9">
         <v>0.5</v>
       </c>
-      <c r="K71" s="9" t="s">
+      <c r="K71" s="9"/>
+      <c r="L71" s="9" t="s">
         <v>117</v>
       </c>
-      <c r="L71" s="4" t="s">
+      <c r="M71" s="4" t="s">
         <v>132</v>
       </c>
     </row>
-    <row r="72" spans="1:12" ht="34" x14ac:dyDescent="0.2">
+    <row r="72" spans="1:13" ht="34" x14ac:dyDescent="0.2">
       <c r="A72" s="5">
         <v>44284</v>
       </c>
@@ -4481,11 +4547,12 @@
       <c r="J72" s="9">
         <v>0.5</v>
       </c>
-      <c r="L72" s="4" t="s">
+      <c r="K72" s="9"/>
+      <c r="M72" s="4" t="s">
         <v>172</v>
       </c>
     </row>
-    <row r="73" spans="1:12" ht="51" x14ac:dyDescent="0.2">
+    <row r="73" spans="1:13" ht="51" x14ac:dyDescent="0.2">
       <c r="A73" s="5">
         <v>44284</v>
       </c>
@@ -4516,11 +4583,12 @@
       <c r="J73" s="9">
         <v>0.5</v>
       </c>
-      <c r="L73" s="4" t="s">
+      <c r="K73" s="9"/>
+      <c r="M73" s="4" t="s">
         <v>176</v>
       </c>
     </row>
-    <row r="74" spans="1:12" ht="51" x14ac:dyDescent="0.2">
+    <row r="74" spans="1:13" ht="51" x14ac:dyDescent="0.2">
       <c r="A74" s="5">
         <v>44284</v>
       </c>
@@ -4551,11 +4619,12 @@
       <c r="J74" s="9">
         <v>0.5</v>
       </c>
-      <c r="L74" s="4" t="s">
+      <c r="K74" s="9"/>
+      <c r="M74" s="4" t="s">
         <v>175</v>
       </c>
     </row>
-    <row r="75" spans="1:12" ht="51" x14ac:dyDescent="0.2">
+    <row r="75" spans="1:13" ht="51" x14ac:dyDescent="0.2">
       <c r="A75" s="5">
         <v>44284</v>
       </c>
@@ -4586,11 +4655,12 @@
       <c r="J75" s="9">
         <v>0.5</v>
       </c>
-      <c r="L75" s="4" t="s">
+      <c r="K75" s="9"/>
+      <c r="M75" s="4" t="s">
         <v>174</v>
       </c>
     </row>
-    <row r="76" spans="1:12" ht="51" x14ac:dyDescent="0.2">
+    <row r="76" spans="1:13" ht="51" x14ac:dyDescent="0.2">
       <c r="A76" s="5">
         <v>44285</v>
       </c>
@@ -4621,14 +4691,15 @@
       <c r="J76" s="9">
         <v>0.5</v>
       </c>
-      <c r="K76" t="s">
+      <c r="K76" s="9"/>
+      <c r="L76" t="s">
         <v>117</v>
       </c>
-      <c r="L76" s="4" t="s">
+      <c r="M76" s="4" t="s">
         <v>170</v>
       </c>
     </row>
-    <row r="77" spans="1:12" s="11" customFormat="1" ht="17" x14ac:dyDescent="0.2">
+    <row r="77" spans="1:13" s="11" customFormat="1" ht="17" x14ac:dyDescent="0.2">
       <c r="A77" s="39">
         <v>44285</v>
       </c>
@@ -4659,14 +4730,15 @@
       <c r="J77" s="14">
         <v>0.5</v>
       </c>
-      <c r="K77" s="11" t="s">
+      <c r="K77" s="14"/>
+      <c r="L77" s="11" t="s">
         <v>116</v>
       </c>
-      <c r="L77" s="12" t="s">
+      <c r="M77" s="12" t="s">
         <v>156</v>
       </c>
     </row>
-    <row r="78" spans="1:12" s="11" customFormat="1" ht="17" x14ac:dyDescent="0.2">
+    <row r="78" spans="1:13" s="11" customFormat="1" ht="17" x14ac:dyDescent="0.2">
       <c r="A78" s="39">
         <v>44285</v>
       </c>
@@ -4697,14 +4769,15 @@
       <c r="J78" s="14">
         <v>0.5</v>
       </c>
-      <c r="K78" s="11" t="s">
+      <c r="K78" s="14"/>
+      <c r="L78" s="11" t="s">
         <v>116</v>
       </c>
-      <c r="L78" s="12" t="s">
+      <c r="M78" s="12" t="s">
         <v>157</v>
       </c>
     </row>
-    <row r="79" spans="1:12" s="36" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="79" spans="1:13" s="36" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A79" s="41">
         <v>44285</v>
       </c>
@@ -4735,14 +4808,15 @@
       <c r="J79" s="35">
         <v>0.5</v>
       </c>
-      <c r="K79" s="36" t="s">
+      <c r="K79" s="35"/>
+      <c r="L79" s="36" t="s">
         <v>117</v>
       </c>
-      <c r="L79" s="42" t="s">
+      <c r="M79" s="42" t="s">
         <v>171</v>
       </c>
     </row>
-    <row r="80" spans="1:12" s="11" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="80" spans="1:13" s="11" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A80" s="39">
         <v>44285</v>
       </c>
@@ -4773,11 +4847,12 @@
       <c r="J80" s="14">
         <v>0.5</v>
       </c>
-      <c r="K80" s="11" t="s">
+      <c r="K80" s="14"/>
+      <c r="L80" s="11" t="s">
         <v>116</v>
       </c>
     </row>
-    <row r="81" spans="1:12" s="11" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="81" spans="1:13" s="11" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A81" s="39">
         <v>44285</v>
       </c>
@@ -4808,11 +4883,12 @@
       <c r="J81" s="14">
         <v>0.5</v>
       </c>
-      <c r="K81" s="11" t="s">
+      <c r="K81" s="14"/>
+      <c r="L81" s="11" t="s">
         <v>116</v>
       </c>
     </row>
-    <row r="82" spans="1:12" s="11" customFormat="1" ht="51" x14ac:dyDescent="0.2">
+    <row r="82" spans="1:13" s="11" customFormat="1" ht="51" x14ac:dyDescent="0.2">
       <c r="A82" s="39">
         <v>44286</v>
       </c>
@@ -4843,14 +4919,15 @@
       <c r="J82" s="14">
         <v>0.5</v>
       </c>
-      <c r="K82" s="11" t="s">
+      <c r="K82" s="14"/>
+      <c r="L82" s="11" t="s">
         <v>116</v>
       </c>
-      <c r="L82" s="12" t="s">
+      <c r="M82" s="12" t="s">
         <v>177</v>
       </c>
     </row>
-    <row r="83" spans="1:12" s="11" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="83" spans="1:13" s="11" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A83" s="39">
         <v>44286</v>
       </c>
@@ -4881,14 +4958,15 @@
       <c r="J83" s="14">
         <v>0.5</v>
       </c>
-      <c r="K83" s="11" t="s">
+      <c r="K83" s="14"/>
+      <c r="L83" s="11" t="s">
         <v>116</v>
       </c>
-      <c r="L83" s="43" t="s">
+      <c r="M83" s="43" t="s">
         <v>178</v>
       </c>
     </row>
-    <row r="84" spans="1:12" s="11" customFormat="1" ht="34" x14ac:dyDescent="0.2">
+    <row r="84" spans="1:13" s="11" customFormat="1" ht="34" x14ac:dyDescent="0.2">
       <c r="A84" s="39">
         <v>44286</v>
       </c>
@@ -4919,14 +4997,15 @@
       <c r="J84" s="14">
         <v>0.5</v>
       </c>
-      <c r="K84" s="11" t="s">
+      <c r="K84" s="14"/>
+      <c r="L84" s="11" t="s">
         <v>116</v>
       </c>
-      <c r="L84" s="12" t="s">
+      <c r="M84" s="12" t="s">
         <v>193</v>
       </c>
     </row>
-    <row r="85" spans="1:12" s="11" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="85" spans="1:13" s="11" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A85" s="39">
         <v>44286</v>
       </c>
@@ -4957,14 +5036,15 @@
       <c r="J85" s="14">
         <v>0.5</v>
       </c>
-      <c r="K85" s="11" t="s">
+      <c r="K85" s="14"/>
+      <c r="L85" s="11" t="s">
         <v>116</v>
       </c>
-      <c r="L85" s="43" t="s">
+      <c r="M85" s="43" t="s">
         <v>194</v>
       </c>
     </row>
-    <row r="86" spans="1:12" s="36" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="86" spans="1:13" s="36" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A86" s="41">
         <v>44286</v>
       </c>
@@ -4995,14 +5075,15 @@
       <c r="J86" s="35">
         <v>0.5</v>
       </c>
-      <c r="K86" s="36" t="s">
+      <c r="K86" s="35"/>
+      <c r="L86" s="36" t="s">
         <v>122</v>
       </c>
-      <c r="L86" s="42" t="s">
+      <c r="M86" s="42" t="s">
         <v>210</v>
       </c>
     </row>
-    <row r="87" spans="1:12" ht="51" x14ac:dyDescent="0.2">
+    <row r="87" spans="1:13" ht="51" x14ac:dyDescent="0.2">
       <c r="A87" s="5">
         <v>44286</v>
       </c>
@@ -5033,14 +5114,15 @@
       <c r="J87" s="35">
         <v>0.5</v>
       </c>
-      <c r="K87" s="36" t="s">
+      <c r="K87" s="35"/>
+      <c r="L87" s="36" t="s">
         <v>117</v>
       </c>
-      <c r="L87" s="4" t="s">
+      <c r="M87" s="4" t="s">
         <v>195</v>
       </c>
     </row>
-    <row r="88" spans="1:12" s="17" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="88" spans="1:13" s="17" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A88" s="15">
         <v>44286</v>
       </c>
@@ -5071,14 +5153,15 @@
       <c r="J88" s="16">
         <v>0.5</v>
       </c>
-      <c r="K88" s="17" t="s">
+      <c r="K88" s="16"/>
+      <c r="L88" s="17" t="s">
         <v>116</v>
       </c>
-      <c r="L88" s="46" t="s">
+      <c r="M88" s="46" t="s">
         <v>196</v>
       </c>
     </row>
-    <row r="89" spans="1:12" s="17" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="89" spans="1:13" s="17" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A89" s="15">
         <v>44286</v>
       </c>
@@ -5109,11 +5192,12 @@
       <c r="J89" s="16">
         <v>0.5</v>
       </c>
-      <c r="K89" s="17" t="s">
+      <c r="K89" s="16"/>
+      <c r="L89" s="17" t="s">
         <v>116</v>
       </c>
     </row>
-    <row r="90" spans="1:12" ht="34" x14ac:dyDescent="0.2">
+    <row r="90" spans="1:13" ht="34" x14ac:dyDescent="0.2">
       <c r="A90" s="5">
         <v>44286</v>
       </c>
@@ -5144,14 +5228,15 @@
       <c r="J90" s="9">
         <v>0.5</v>
       </c>
-      <c r="K90" s="9" t="s">
+      <c r="K90" s="9"/>
+      <c r="L90" s="9" t="s">
         <v>117</v>
       </c>
-      <c r="L90" s="4" t="s">
+      <c r="M90" s="4" t="s">
         <v>198</v>
       </c>
     </row>
-    <row r="91" spans="1:12" s="24" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="91" spans="1:13" s="24" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A91" s="49">
         <v>44288</v>
       </c>
@@ -5182,14 +5267,15 @@
       <c r="J91" s="23">
         <v>0.5</v>
       </c>
-      <c r="K91" s="24" t="s">
+      <c r="K91" s="23"/>
+      <c r="L91" s="24" t="s">
         <v>116</v>
       </c>
-      <c r="L91" s="38" t="s">
+      <c r="M91" s="38" t="s">
         <v>211</v>
       </c>
     </row>
-    <row r="92" spans="1:12" s="24" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="92" spans="1:13" s="24" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A92" s="49">
         <v>44288</v>
       </c>
@@ -5220,11 +5306,12 @@
       <c r="J92" s="23">
         <v>0.5</v>
       </c>
-      <c r="K92" s="24" t="s">
+      <c r="K92" s="23"/>
+      <c r="L92" s="24" t="s">
         <v>116</v>
       </c>
     </row>
-    <row r="93" spans="1:12" s="24" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="93" spans="1:13" s="24" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A93" s="49">
         <v>44288</v>
       </c>
@@ -5255,11 +5342,12 @@
       <c r="J93" s="23">
         <v>0.5</v>
       </c>
-      <c r="K93" s="24" t="s">
+      <c r="K93" s="23"/>
+      <c r="L93" s="24" t="s">
         <v>116</v>
       </c>
     </row>
-    <row r="94" spans="1:12" ht="51" x14ac:dyDescent="0.2">
+    <row r="94" spans="1:13" ht="51" x14ac:dyDescent="0.2">
       <c r="A94" s="5">
         <v>44288</v>
       </c>
@@ -5290,14 +5378,15 @@
       <c r="J94" s="9">
         <v>0.5</v>
       </c>
-      <c r="K94" t="s">
+      <c r="K94" s="9"/>
+      <c r="L94" t="s">
         <v>117</v>
       </c>
-      <c r="L94" s="4" t="s">
+      <c r="M94" s="4" t="s">
         <v>212</v>
       </c>
     </row>
-    <row r="95" spans="1:12" s="17" customFormat="1" ht="68" x14ac:dyDescent="0.2">
+    <row r="95" spans="1:13" s="17" customFormat="1" ht="68" x14ac:dyDescent="0.2">
       <c r="A95" s="50">
         <v>44288</v>
       </c>
@@ -5328,14 +5417,15 @@
       <c r="J95" s="16">
         <v>0.5</v>
       </c>
-      <c r="K95" s="17" t="s">
+      <c r="K95" s="16"/>
+      <c r="L95" s="17" t="s">
         <v>116</v>
       </c>
-      <c r="L95" s="28" t="s">
+      <c r="M95" s="28" t="s">
         <v>213</v>
       </c>
     </row>
-    <row r="96" spans="1:12" s="17" customFormat="1" ht="34" x14ac:dyDescent="0.2">
+    <row r="96" spans="1:13" s="17" customFormat="1" ht="34" x14ac:dyDescent="0.2">
       <c r="A96" s="50">
         <v>44288</v>
       </c>
@@ -5366,14 +5456,15 @@
       <c r="J96" s="16">
         <v>0.5</v>
       </c>
-      <c r="K96" s="17" t="s">
+      <c r="K96" s="16"/>
+      <c r="L96" s="17" t="s">
         <v>116</v>
       </c>
-      <c r="L96" s="28" t="s">
+      <c r="M96" s="28" t="s">
         <v>214</v>
       </c>
     </row>
-    <row r="97" spans="1:12" ht="51" x14ac:dyDescent="0.2">
+    <row r="97" spans="1:13" ht="51" x14ac:dyDescent="0.2">
       <c r="A97" s="5">
         <v>44288</v>
       </c>
@@ -5404,14 +5495,15 @@
       <c r="J97" s="9">
         <v>0.5</v>
       </c>
-      <c r="K97" t="s">
+      <c r="K97" s="9"/>
+      <c r="L97" t="s">
         <v>117</v>
       </c>
-      <c r="L97" s="4" t="s">
+      <c r="M97" s="4" t="s">
         <v>215</v>
       </c>
     </row>
-    <row r="98" spans="1:12" s="17" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="98" spans="1:13" s="17" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A98" s="50">
         <v>44288</v>
       </c>
@@ -5442,11 +5534,12 @@
       <c r="J98" s="16">
         <v>0.5</v>
       </c>
-      <c r="K98" s="17" t="s">
+      <c r="K98" s="16"/>
+      <c r="L98" s="17" t="s">
         <v>116</v>
       </c>
     </row>
-    <row r="99" spans="1:12" s="17" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="99" spans="1:13" s="17" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A99" s="50">
         <v>44288</v>
       </c>
@@ -5477,11 +5570,12 @@
       <c r="J99" s="16">
         <v>0.5</v>
       </c>
-      <c r="K99" s="17" t="s">
+      <c r="K99" s="16"/>
+      <c r="L99" s="17" t="s">
         <v>116</v>
       </c>
     </row>
-    <row r="100" spans="1:12" ht="34" x14ac:dyDescent="0.2">
+    <row r="100" spans="1:13" ht="34" x14ac:dyDescent="0.2">
       <c r="A100" s="5">
         <v>44288</v>
       </c>
@@ -5512,14 +5606,15 @@
       <c r="J100" s="9">
         <v>0.5</v>
       </c>
-      <c r="K100" t="s">
+      <c r="K100" s="9"/>
+      <c r="L100" t="s">
         <v>117</v>
       </c>
-      <c r="L100" s="4" t="s">
+      <c r="M100" s="4" t="s">
         <v>216</v>
       </c>
     </row>
-    <row r="101" spans="1:12" s="20" customFormat="1" ht="51" x14ac:dyDescent="0.2">
+    <row r="101" spans="1:13" s="20" customFormat="1" ht="51" x14ac:dyDescent="0.2">
       <c r="A101" s="18">
         <v>44289</v>
       </c>
@@ -5550,14 +5645,15 @@
       <c r="J101" s="51">
         <v>0.5</v>
       </c>
-      <c r="K101" s="20" t="s">
+      <c r="K101" s="51"/>
+      <c r="L101" s="20" t="s">
         <v>116</v>
       </c>
-      <c r="L101" s="21" t="s">
+      <c r="M101" s="21" t="s">
         <v>227</v>
       </c>
     </row>
-    <row r="102" spans="1:12" s="20" customFormat="1" ht="34" x14ac:dyDescent="0.2">
+    <row r="102" spans="1:13" s="20" customFormat="1" ht="34" x14ac:dyDescent="0.2">
       <c r="A102" s="18">
         <v>44289</v>
       </c>
@@ -5588,14 +5684,15 @@
       <c r="J102" s="51">
         <v>0.5</v>
       </c>
-      <c r="K102" s="20" t="s">
+      <c r="K102" s="51"/>
+      <c r="L102" s="20" t="s">
         <v>116</v>
       </c>
-      <c r="L102" s="21" t="s">
+      <c r="M102" s="21" t="s">
         <v>228</v>
       </c>
     </row>
-    <row r="103" spans="1:12" ht="51" x14ac:dyDescent="0.2">
+    <row r="103" spans="1:13" ht="51" x14ac:dyDescent="0.2">
       <c r="A103" s="5">
         <v>44289</v>
       </c>
@@ -5626,14 +5723,15 @@
       <c r="J103" s="9">
         <v>0.5</v>
       </c>
-      <c r="K103" s="36" t="s">
+      <c r="K103" s="9"/>
+      <c r="L103" s="36" t="s">
         <v>117</v>
       </c>
-      <c r="L103" s="4" t="s">
+      <c r="M103" s="4" t="s">
         <v>229</v>
       </c>
     </row>
-    <row r="104" spans="1:12" ht="51" x14ac:dyDescent="0.2">
+    <row r="104" spans="1:13" ht="51" x14ac:dyDescent="0.2">
       <c r="A104" s="5">
         <v>44289</v>
       </c>
@@ -5664,14 +5762,15 @@
       <c r="J104" s="9">
         <v>0.5</v>
       </c>
-      <c r="K104" s="36" t="s">
+      <c r="K104" s="9"/>
+      <c r="L104" s="36" t="s">
         <v>117</v>
       </c>
-      <c r="L104" s="4" t="s">
+      <c r="M104" s="4" t="s">
         <v>230</v>
       </c>
     </row>
-    <row r="105" spans="1:12" s="20" customFormat="1" ht="17" x14ac:dyDescent="0.2">
+    <row r="105" spans="1:13" s="20" customFormat="1" ht="17" x14ac:dyDescent="0.2">
       <c r="A105" s="18">
         <v>44289</v>
       </c>
@@ -5702,14 +5801,15 @@
       <c r="J105" s="51">
         <v>0.5</v>
       </c>
-      <c r="K105" s="20" t="s">
+      <c r="K105" s="51"/>
+      <c r="L105" s="20" t="s">
         <v>116</v>
       </c>
-      <c r="L105" s="21" t="s">
+      <c r="M105" s="21" t="s">
         <v>231</v>
       </c>
     </row>
-    <row r="106" spans="1:12" s="20" customFormat="1" ht="17" x14ac:dyDescent="0.2">
+    <row r="106" spans="1:13" s="20" customFormat="1" ht="17" x14ac:dyDescent="0.2">
       <c r="A106" s="18">
         <v>44289</v>
       </c>
@@ -5740,14 +5840,15 @@
       <c r="J106" s="51">
         <v>0.5</v>
       </c>
-      <c r="K106" s="20" t="s">
+      <c r="K106" s="51"/>
+      <c r="L106" s="20" t="s">
         <v>116</v>
       </c>
-      <c r="L106" s="21" t="s">
+      <c r="M106" s="21" t="s">
         <v>232</v>
       </c>
     </row>
-    <row r="107" spans="1:12" s="17" customFormat="1" ht="17" x14ac:dyDescent="0.2">
+    <row r="107" spans="1:13" s="17" customFormat="1" ht="17" x14ac:dyDescent="0.2">
       <c r="A107" s="50">
         <v>44289</v>
       </c>
@@ -5778,14 +5879,15 @@
       <c r="J107" s="16">
         <v>0.5</v>
       </c>
-      <c r="K107" s="17" t="s">
+      <c r="K107" s="16"/>
+      <c r="L107" s="17" t="s">
         <v>116</v>
       </c>
-      <c r="L107" s="28" t="s">
+      <c r="M107" s="28" t="s">
         <v>233</v>
       </c>
     </row>
-    <row r="108" spans="1:12" s="17" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="108" spans="1:13" s="17" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A108" s="50">
         <v>44289</v>
       </c>
@@ -5816,11 +5918,12 @@
       <c r="J108" s="16">
         <v>0.5</v>
       </c>
-      <c r="K108" s="17" t="s">
+      <c r="K108" s="16"/>
+      <c r="L108" s="17" t="s">
         <v>116</v>
       </c>
     </row>
-    <row r="109" spans="1:12" ht="34" x14ac:dyDescent="0.2">
+    <row r="109" spans="1:13" ht="34" x14ac:dyDescent="0.2">
       <c r="A109" s="5">
         <v>44289</v>
       </c>
@@ -5851,14 +5954,15 @@
       <c r="J109" s="9">
         <v>0.5</v>
       </c>
-      <c r="K109" s="36" t="s">
+      <c r="K109" s="9"/>
+      <c r="L109" s="36" t="s">
         <v>117</v>
       </c>
-      <c r="L109" s="4" t="s">
+      <c r="M109" s="4" t="s">
         <v>234</v>
       </c>
     </row>
-    <row r="110" spans="1:12" ht="102" x14ac:dyDescent="0.2">
+    <row r="110" spans="1:13" ht="102" x14ac:dyDescent="0.2">
       <c r="A110" s="5">
         <v>44289</v>
       </c>
@@ -5889,11 +5993,12 @@
       <c r="J110" s="9">
         <v>0.5</v>
       </c>
-      <c r="L110" s="4" t="s">
+      <c r="K110" s="9"/>
+      <c r="M110" s="4" t="s">
         <v>236</v>
       </c>
     </row>
-    <row r="111" spans="1:12" ht="17" x14ac:dyDescent="0.2">
+    <row r="111" spans="1:13" ht="17" x14ac:dyDescent="0.2">
       <c r="A111" s="5">
         <v>44289</v>
       </c>
@@ -5924,11 +6029,12 @@
       <c r="J111" s="9">
         <v>0.5</v>
       </c>
-      <c r="L111" s="4" t="s">
+      <c r="K111" s="9"/>
+      <c r="M111" s="4" t="s">
         <v>237</v>
       </c>
     </row>
-    <row r="112" spans="1:12" s="55" customFormat="1" ht="68" x14ac:dyDescent="0.2">
+    <row r="112" spans="1:13" s="55" customFormat="1" ht="68" x14ac:dyDescent="0.2">
       <c r="A112" s="52">
         <v>44289</v>
       </c>
@@ -5959,11 +6065,12 @@
       <c r="J112" s="54">
         <v>0.5</v>
       </c>
-      <c r="L112" s="56" t="s">
+      <c r="K112" s="54"/>
+      <c r="M112" s="56" t="s">
         <v>259</v>
       </c>
     </row>
-    <row r="113" spans="1:12" ht="238" x14ac:dyDescent="0.2">
+    <row r="113" spans="1:13" ht="238" x14ac:dyDescent="0.2">
       <c r="A113" s="5">
         <v>44289</v>
       </c>
@@ -5994,11 +6101,12 @@
       <c r="J113" s="9">
         <v>0.5</v>
       </c>
-      <c r="L113" s="4" t="s">
+      <c r="K113" s="9"/>
+      <c r="M113" s="4" t="s">
         <v>238</v>
       </c>
     </row>
-    <row r="114" spans="1:12" ht="102" x14ac:dyDescent="0.2">
+    <row r="114" spans="1:13" ht="102" x14ac:dyDescent="0.2">
       <c r="A114" s="5">
         <v>44289</v>
       </c>
@@ -6029,11 +6137,12 @@
       <c r="J114" s="9">
         <v>0.5</v>
       </c>
-      <c r="L114" s="4" t="s">
+      <c r="K114" s="9"/>
+      <c r="M114" s="4" t="s">
         <v>260</v>
       </c>
     </row>
-    <row r="115" spans="1:12" ht="51" x14ac:dyDescent="0.2">
+    <row r="115" spans="1:13" ht="51" x14ac:dyDescent="0.2">
       <c r="A115" s="5">
         <v>44289</v>
       </c>
@@ -6064,11 +6173,12 @@
       <c r="J115" s="9">
         <v>0.5</v>
       </c>
-      <c r="L115" s="4" t="s">
+      <c r="K115" s="9"/>
+      <c r="M115" s="4" t="s">
         <v>239</v>
       </c>
     </row>
-    <row r="116" spans="1:12" s="55" customFormat="1" ht="227" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="116" spans="1:13" s="55" customFormat="1" ht="227" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A116" s="52">
         <v>44290</v>
       </c>
@@ -6099,11 +6209,12 @@
       <c r="J116" s="54">
         <v>0.5</v>
       </c>
-      <c r="L116" s="56" t="s">
+      <c r="K116" s="54"/>
+      <c r="M116" s="56" t="s">
         <v>263</v>
       </c>
     </row>
-    <row r="117" spans="1:12" ht="170" x14ac:dyDescent="0.2">
+    <row r="117" spans="1:13" ht="170" x14ac:dyDescent="0.2">
       <c r="A117" s="5">
         <v>44290</v>
       </c>
@@ -6134,11 +6245,12 @@
       <c r="J117" s="9">
         <v>0.5</v>
       </c>
-      <c r="L117" s="4" t="s">
+      <c r="K117" s="9"/>
+      <c r="M117" s="4" t="s">
         <v>264</v>
       </c>
     </row>
-    <row r="118" spans="1:12" s="55" customFormat="1" ht="238" x14ac:dyDescent="0.2">
+    <row r="118" spans="1:13" s="55" customFormat="1" ht="238" x14ac:dyDescent="0.2">
       <c r="A118" s="52">
         <v>44290</v>
       </c>
@@ -6169,11 +6281,12 @@
       <c r="J118" s="54">
         <v>0.5</v>
       </c>
-      <c r="L118" s="56" t="s">
+      <c r="K118" s="54"/>
+      <c r="M118" s="56" t="s">
         <v>265</v>
       </c>
     </row>
-    <row r="119" spans="1:12" ht="51" x14ac:dyDescent="0.2">
+    <row r="119" spans="1:13" ht="51" x14ac:dyDescent="0.2">
       <c r="A119" s="5">
         <v>44290</v>
       </c>
@@ -6204,11 +6317,12 @@
       <c r="J119" s="9">
         <v>0.5</v>
       </c>
-      <c r="L119" s="4" t="s">
+      <c r="K119" s="9"/>
+      <c r="M119" s="4" t="s">
         <v>267</v>
       </c>
     </row>
-    <row r="120" spans="1:12" ht="68" x14ac:dyDescent="0.2">
+    <row r="120" spans="1:13" ht="68" x14ac:dyDescent="0.2">
       <c r="A120" s="5">
         <v>44290</v>
       </c>
@@ -6239,11 +6353,12 @@
       <c r="J120" s="9">
         <v>0.5</v>
       </c>
-      <c r="L120" s="4" t="s">
+      <c r="K120" s="9"/>
+      <c r="M120" s="4" t="s">
         <v>268</v>
       </c>
     </row>
-    <row r="121" spans="1:12" ht="68" x14ac:dyDescent="0.2">
+    <row r="121" spans="1:13" ht="68" x14ac:dyDescent="0.2">
       <c r="A121" s="5">
         <v>44290</v>
       </c>
@@ -6274,11 +6389,12 @@
       <c r="J121" s="9">
         <v>0.5</v>
       </c>
-      <c r="L121" s="4" t="s">
+      <c r="K121" s="9"/>
+      <c r="M121" s="4" t="s">
         <v>269</v>
       </c>
     </row>
-    <row r="122" spans="1:12" ht="85" x14ac:dyDescent="0.2">
+    <row r="122" spans="1:13" ht="85" x14ac:dyDescent="0.2">
       <c r="A122" s="5">
         <v>44290</v>
       </c>
@@ -6309,11 +6425,12 @@
       <c r="J122" s="9">
         <v>0.5</v>
       </c>
-      <c r="L122" s="4" t="s">
+      <c r="K122" s="9"/>
+      <c r="M122" s="4" t="s">
         <v>270</v>
       </c>
     </row>
-    <row r="123" spans="1:12" ht="51" x14ac:dyDescent="0.2">
+    <row r="123" spans="1:13" ht="51" x14ac:dyDescent="0.2">
       <c r="A123" s="5">
         <v>44290</v>
       </c>
@@ -6344,11 +6461,12 @@
       <c r="J123" s="9">
         <v>0.5</v>
       </c>
-      <c r="L123" s="4" t="s">
+      <c r="K123" s="9"/>
+      <c r="M123" s="4" t="s">
         <v>271</v>
       </c>
     </row>
-    <row r="124" spans="1:12" ht="51" x14ac:dyDescent="0.2">
+    <row r="124" spans="1:13" ht="51" x14ac:dyDescent="0.2">
       <c r="A124" s="5">
         <v>44290</v>
       </c>
@@ -6379,11 +6497,12 @@
       <c r="J124" s="9">
         <v>0.5</v>
       </c>
-      <c r="L124" s="4" t="s">
+      <c r="K124" s="9"/>
+      <c r="M124" s="4" t="s">
         <v>272</v>
       </c>
     </row>
-    <row r="125" spans="1:12" ht="34" x14ac:dyDescent="0.2">
+    <row r="125" spans="1:13" ht="34" x14ac:dyDescent="0.2">
       <c r="A125" s="5">
         <v>44290</v>
       </c>
@@ -6414,11 +6533,12 @@
       <c r="J125" s="9">
         <v>0.5</v>
       </c>
-      <c r="L125" s="4" t="s">
+      <c r="K125" s="9"/>
+      <c r="M125" s="4" t="s">
         <v>273</v>
       </c>
     </row>
-    <row r="126" spans="1:12" ht="34" x14ac:dyDescent="0.2">
+    <row r="126" spans="1:13" ht="34" x14ac:dyDescent="0.2">
       <c r="A126" s="5">
         <v>44292</v>
       </c>
@@ -6449,11 +6569,12 @@
       <c r="J126" s="9">
         <v>0.5</v>
       </c>
-      <c r="L126" s="4" t="s">
+      <c r="K126" s="9"/>
+      <c r="M126" s="4" t="s">
         <v>285</v>
       </c>
     </row>
-    <row r="127" spans="1:12" ht="85" x14ac:dyDescent="0.2">
+    <row r="127" spans="1:13" ht="85" x14ac:dyDescent="0.2">
       <c r="A127" s="5">
         <v>44292</v>
       </c>
@@ -6484,11 +6605,12 @@
       <c r="J127" s="9">
         <v>0.5</v>
       </c>
-      <c r="L127" s="4" t="s">
+      <c r="K127" s="9"/>
+      <c r="M127" s="4" t="s">
         <v>286</v>
       </c>
     </row>
-    <row r="128" spans="1:12" ht="85" x14ac:dyDescent="0.2">
+    <row r="128" spans="1:13" ht="85" x14ac:dyDescent="0.2">
       <c r="A128" s="5">
         <v>44292</v>
       </c>
@@ -6519,11 +6641,12 @@
       <c r="J128" s="9">
         <v>0.5</v>
       </c>
-      <c r="L128" s="4" t="s">
+      <c r="K128" s="9"/>
+      <c r="M128" s="4" t="s">
         <v>287</v>
       </c>
     </row>
-    <row r="129" spans="1:12" ht="17" x14ac:dyDescent="0.2">
+    <row r="129" spans="1:13" ht="17" x14ac:dyDescent="0.2">
       <c r="A129" s="5">
         <v>44292</v>
       </c>
@@ -6554,11 +6677,12 @@
       <c r="J129" s="9">
         <v>0.5</v>
       </c>
-      <c r="L129" s="4" t="s">
+      <c r="K129" s="9"/>
+      <c r="M129" s="4" t="s">
         <v>288</v>
       </c>
     </row>
-    <row r="130" spans="1:12" ht="51" x14ac:dyDescent="0.2">
+    <row r="130" spans="1:13" ht="51" x14ac:dyDescent="0.2">
       <c r="A130" s="5">
         <v>44292</v>
       </c>
@@ -6589,11 +6713,12 @@
       <c r="J130" s="9">
         <v>0.5</v>
       </c>
-      <c r="L130" s="4" t="s">
+      <c r="K130" s="9"/>
+      <c r="M130" s="4" t="s">
         <v>289</v>
       </c>
     </row>
-    <row r="131" spans="1:12" ht="51" x14ac:dyDescent="0.2">
+    <row r="131" spans="1:13" ht="51" x14ac:dyDescent="0.2">
       <c r="A131" s="5">
         <v>44292</v>
       </c>
@@ -6624,11 +6749,12 @@
       <c r="J131" s="9">
         <v>0.5</v>
       </c>
-      <c r="L131" s="4" t="s">
+      <c r="K131" s="9"/>
+      <c r="M131" s="4" t="s">
         <v>290</v>
       </c>
     </row>
-    <row r="132" spans="1:12" ht="356" x14ac:dyDescent="0.2">
+    <row r="132" spans="1:13" ht="356" x14ac:dyDescent="0.2">
       <c r="A132" s="5">
         <v>44293</v>
       </c>
@@ -6659,11 +6785,12 @@
       <c r="J132" s="9">
         <v>0.5</v>
       </c>
-      <c r="L132" s="57" t="s">
+      <c r="K132" s="9"/>
+      <c r="M132" s="57" t="s">
         <v>291</v>
       </c>
     </row>
-    <row r="133" spans="1:12" ht="255" x14ac:dyDescent="0.2">
+    <row r="133" spans="1:13" ht="255" x14ac:dyDescent="0.2">
       <c r="A133" s="5">
         <v>44293</v>
       </c>
@@ -6694,11 +6821,12 @@
       <c r="J133" s="9">
         <v>0.5</v>
       </c>
-      <c r="L133" s="57" t="s">
+      <c r="K133" s="9"/>
+      <c r="M133" s="57" t="s">
         <v>292</v>
       </c>
     </row>
-    <row r="134" spans="1:12" ht="68" x14ac:dyDescent="0.2">
+    <row r="134" spans="1:13" ht="68" x14ac:dyDescent="0.2">
       <c r="A134" s="5">
         <v>44293</v>
       </c>
@@ -6729,11 +6857,12 @@
       <c r="J134" s="9">
         <v>0.5</v>
       </c>
-      <c r="L134" s="57" t="s">
+      <c r="K134" s="9"/>
+      <c r="M134" s="57" t="s">
         <v>293</v>
       </c>
     </row>
-    <row r="135" spans="1:12" ht="34" x14ac:dyDescent="0.2">
+    <row r="135" spans="1:13" ht="34" x14ac:dyDescent="0.2">
       <c r="A135" s="5">
         <v>44293</v>
       </c>
@@ -6764,11 +6893,12 @@
       <c r="J135" s="9">
         <v>0.5</v>
       </c>
-      <c r="L135" s="57" t="s">
+      <c r="K135" s="9"/>
+      <c r="M135" s="57" t="s">
         <v>294</v>
       </c>
     </row>
-    <row r="136" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="136" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A136" s="5">
         <v>44293</v>
       </c>
@@ -6799,8 +6929,9 @@
       <c r="J136" s="9">
         <v>0.5</v>
       </c>
-    </row>
-    <row r="137" spans="1:12" ht="34" x14ac:dyDescent="0.2">
+      <c r="K136" s="9"/>
+    </row>
+    <row r="137" spans="1:13" ht="34" x14ac:dyDescent="0.2">
       <c r="A137" s="5">
         <v>44293</v>
       </c>
@@ -6831,11 +6962,12 @@
       <c r="J137" s="9">
         <v>0.5</v>
       </c>
-      <c r="L137" s="57" t="s">
+      <c r="K137" s="9"/>
+      <c r="M137" s="57" t="s">
         <v>295</v>
       </c>
     </row>
-    <row r="138" spans="1:12" ht="17" x14ac:dyDescent="0.2">
+    <row r="138" spans="1:13" ht="17" x14ac:dyDescent="0.2">
       <c r="A138" s="5">
         <v>44293</v>
       </c>
@@ -6866,11 +6998,12 @@
       <c r="J138" s="9">
         <v>0.5</v>
       </c>
-      <c r="L138" s="57" t="s">
+      <c r="K138" s="9"/>
+      <c r="M138" s="57" t="s">
         <v>296</v>
       </c>
     </row>
-    <row r="139" spans="1:12" ht="68" x14ac:dyDescent="0.2">
+    <row r="139" spans="1:13" ht="68" x14ac:dyDescent="0.2">
       <c r="A139" s="5">
         <v>44293</v>
       </c>
@@ -6901,11 +7034,12 @@
       <c r="J139" s="9">
         <v>0.5</v>
       </c>
-      <c r="L139" s="57" t="s">
+      <c r="K139" s="9"/>
+      <c r="M139" s="57" t="s">
         <v>297</v>
       </c>
     </row>
-    <row r="140" spans="1:12" ht="34" x14ac:dyDescent="0.2">
+    <row r="140" spans="1:13" ht="34" x14ac:dyDescent="0.2">
       <c r="A140" s="5">
         <v>44294</v>
       </c>
@@ -6936,11 +7070,12 @@
       <c r="J140" s="9">
         <v>0.5</v>
       </c>
-      <c r="L140" s="57" t="s">
+      <c r="K140" s="9"/>
+      <c r="M140" s="57" t="s">
         <v>299</v>
       </c>
     </row>
-    <row r="141" spans="1:12" ht="17" x14ac:dyDescent="0.2">
+    <row r="141" spans="1:13" ht="17" x14ac:dyDescent="0.2">
       <c r="A141" s="5">
         <v>44294</v>
       </c>
@@ -6971,11 +7106,12 @@
       <c r="J141" s="9">
         <v>0.5</v>
       </c>
-      <c r="L141" s="57" t="s">
+      <c r="K141" s="9"/>
+      <c r="M141" s="57" t="s">
         <v>300</v>
       </c>
     </row>
-    <row r="142" spans="1:12" ht="85" x14ac:dyDescent="0.2">
+    <row r="142" spans="1:13" ht="85" x14ac:dyDescent="0.2">
       <c r="A142" s="5">
         <v>44295</v>
       </c>
@@ -7006,11 +7142,14 @@
       <c r="J142" s="9">
         <v>0.5</v>
       </c>
-      <c r="L142" s="57" t="s">
+      <c r="K142" s="9">
+        <v>5</v>
+      </c>
+      <c r="M142" s="57" t="s">
         <v>301</v>
       </c>
     </row>
-    <row r="143" spans="1:12" ht="68" x14ac:dyDescent="0.2">
+    <row r="143" spans="1:13" ht="68" x14ac:dyDescent="0.2">
       <c r="A143" s="5">
         <v>44295</v>
       </c>
@@ -7041,11 +7180,14 @@
       <c r="J143" s="9">
         <v>0.5</v>
       </c>
-      <c r="L143" s="57" t="s">
+      <c r="K143" s="9">
+        <v>5</v>
+      </c>
+      <c r="M143" s="57" t="s">
         <v>302</v>
       </c>
     </row>
-    <row r="144" spans="1:12" ht="17" x14ac:dyDescent="0.2">
+    <row r="144" spans="1:13" ht="17" x14ac:dyDescent="0.2">
       <c r="A144" s="5">
         <v>44295</v>
       </c>
@@ -7076,11 +7218,14 @@
       <c r="J144" s="9">
         <v>0.5</v>
       </c>
-      <c r="L144" s="57" t="s">
+      <c r="K144" s="9">
+        <v>5</v>
+      </c>
+      <c r="M144" s="57" t="s">
         <v>303</v>
       </c>
     </row>
-    <row r="145" spans="1:12" ht="102" x14ac:dyDescent="0.2">
+    <row r="145" spans="1:13" ht="102" x14ac:dyDescent="0.2">
       <c r="A145" s="5">
         <v>44295</v>
       </c>
@@ -7111,11 +7256,14 @@
       <c r="J145" s="9">
         <v>0.5</v>
       </c>
-      <c r="L145" s="57" t="s">
+      <c r="K145" s="9">
+        <v>5</v>
+      </c>
+      <c r="M145" s="57" t="s">
         <v>304</v>
       </c>
     </row>
-    <row r="146" spans="1:12" ht="85" x14ac:dyDescent="0.2">
+    <row r="146" spans="1:13" ht="85" x14ac:dyDescent="0.2">
       <c r="A146" s="5">
         <v>44295</v>
       </c>
@@ -7146,11 +7294,14 @@
       <c r="J146" s="9">
         <v>0.5</v>
       </c>
-      <c r="L146" s="4" t="s">
+      <c r="K146" s="9">
+        <v>5</v>
+      </c>
+      <c r="M146" s="4" t="s">
         <v>305</v>
       </c>
     </row>
-    <row r="147" spans="1:12" ht="17" x14ac:dyDescent="0.2">
+    <row r="147" spans="1:13" ht="17" x14ac:dyDescent="0.2">
       <c r="A147" s="5">
         <v>44295</v>
       </c>
@@ -7181,11 +7332,14 @@
       <c r="J147" s="9">
         <v>0.5</v>
       </c>
-      <c r="L147" s="4" t="s">
+      <c r="K147" s="9">
+        <v>5</v>
+      </c>
+      <c r="M147" s="4" t="s">
         <v>306</v>
       </c>
     </row>
-    <row r="148" spans="1:12" ht="102" x14ac:dyDescent="0.2">
+    <row r="148" spans="1:13" ht="102" x14ac:dyDescent="0.2">
       <c r="A148" s="5">
         <v>44295</v>
       </c>
@@ -7216,11 +7370,14 @@
       <c r="J148" s="9">
         <v>0.5</v>
       </c>
-      <c r="L148" s="4" t="s">
+      <c r="K148" s="9">
+        <v>5</v>
+      </c>
+      <c r="M148" s="4" t="s">
         <v>309</v>
       </c>
     </row>
-    <row r="149" spans="1:12" ht="102" x14ac:dyDescent="0.2">
+    <row r="149" spans="1:13" ht="102" x14ac:dyDescent="0.2">
       <c r="A149" s="5">
         <v>44295</v>
       </c>
@@ -7251,11 +7408,14 @@
       <c r="J149" s="9">
         <v>0.5</v>
       </c>
-      <c r="L149" s="4" t="s">
+      <c r="K149" s="9">
+        <v>5</v>
+      </c>
+      <c r="M149" s="4" t="s">
         <v>310</v>
       </c>
     </row>
-    <row r="150" spans="1:12" ht="51" x14ac:dyDescent="0.2">
+    <row r="150" spans="1:13" ht="51" x14ac:dyDescent="0.2">
       <c r="A150" s="5">
         <v>44295</v>
       </c>
@@ -7286,11 +7446,14 @@
       <c r="J150" s="9">
         <v>0.5</v>
       </c>
-      <c r="L150" s="4" t="s">
+      <c r="K150" s="9">
+        <v>5</v>
+      </c>
+      <c r="M150" s="4" t="s">
         <v>311</v>
       </c>
     </row>
-    <row r="151" spans="1:12" ht="68" x14ac:dyDescent="0.2">
+    <row r="151" spans="1:13" ht="68" x14ac:dyDescent="0.2">
       <c r="A151" s="5">
         <v>44295</v>
       </c>
@@ -7321,253 +7484,540 @@
       <c r="J151" s="9">
         <v>0.5</v>
       </c>
-      <c r="L151" s="4" t="s">
+      <c r="K151" s="9">
+        <v>5</v>
+      </c>
+      <c r="M151" s="4" t="s">
         <v>312</v>
       </c>
     </row>
-    <row r="152" spans="1:12" ht="34" x14ac:dyDescent="0.2">
-      <c r="A152" s="5">
+    <row r="152" spans="1:13" s="61" customFormat="1" ht="34" x14ac:dyDescent="0.2">
+      <c r="A152" s="58">
         <v>44295</v>
       </c>
-      <c r="B152" s="3">
+      <c r="B152" s="59">
         <v>0.6</v>
       </c>
-      <c r="C152" s="9" t="s">
+      <c r="C152" s="60" t="s">
         <v>307</v>
       </c>
-      <c r="D152" t="s">
+      <c r="D152" s="61" t="s">
         <v>326</v>
       </c>
-      <c r="E152" s="9">
+      <c r="E152" s="60">
         <v>1.6</v>
       </c>
-      <c r="F152" s="9">
-        <v>0.04</v>
-      </c>
-      <c r="G152" s="9">
-        <v>4</v>
-      </c>
-      <c r="H152" s="9">
-        <v>1</v>
-      </c>
-      <c r="I152" s="9">
-        <v>0</v>
-      </c>
-      <c r="J152" s="9">
-        <v>0.5</v>
-      </c>
-      <c r="L152" s="4" t="s">
+      <c r="F152" s="60">
+        <v>0.04</v>
+      </c>
+      <c r="G152" s="60">
+        <v>4</v>
+      </c>
+      <c r="H152" s="60">
+        <v>1</v>
+      </c>
+      <c r="I152" s="60">
+        <v>0</v>
+      </c>
+      <c r="J152" s="60">
+        <v>0.5</v>
+      </c>
+      <c r="K152" s="60">
+        <v>5</v>
+      </c>
+      <c r="M152" s="62" t="s">
         <v>313</v>
       </c>
     </row>
-    <row r="153" spans="1:12" ht="34" x14ac:dyDescent="0.2">
-      <c r="A153" s="5">
+    <row r="153" spans="1:13" s="61" customFormat="1" ht="34" x14ac:dyDescent="0.2">
+      <c r="A153" s="58">
         <v>44295</v>
       </c>
-      <c r="B153" s="3">
+      <c r="B153" s="59">
         <v>0.61527777777777781</v>
       </c>
-      <c r="C153" s="9" t="s">
+      <c r="C153" s="60" t="s">
         <v>308</v>
       </c>
-      <c r="D153" t="s">
+      <c r="D153" s="61" t="s">
         <v>325</v>
       </c>
-      <c r="E153" s="9">
+      <c r="E153" s="60">
         <v>1.6</v>
       </c>
-      <c r="F153" s="9">
-        <v>0.04</v>
-      </c>
-      <c r="G153" s="9">
-        <v>4</v>
-      </c>
-      <c r="H153" s="9">
-        <v>1</v>
-      </c>
-      <c r="I153" s="9">
-        <v>0</v>
-      </c>
-      <c r="J153" s="9">
-        <v>0.5</v>
-      </c>
-      <c r="L153" s="4" t="s">
+      <c r="F153" s="60">
+        <v>0.04</v>
+      </c>
+      <c r="G153" s="60">
+        <v>4</v>
+      </c>
+      <c r="H153" s="60">
+        <v>1</v>
+      </c>
+      <c r="I153" s="60">
+        <v>0</v>
+      </c>
+      <c r="J153" s="60">
+        <v>0.5</v>
+      </c>
+      <c r="K153" s="60">
+        <v>5</v>
+      </c>
+      <c r="M153" s="62" t="s">
         <v>314</v>
       </c>
     </row>
-    <row r="154" spans="1:12" ht="85" x14ac:dyDescent="0.2">
-      <c r="A154" s="5">
+    <row r="154" spans="1:13" s="61" customFormat="1" ht="85" x14ac:dyDescent="0.2">
+      <c r="A154" s="58">
         <v>44295</v>
       </c>
-      <c r="B154" s="3">
+      <c r="B154" s="59">
         <v>0.62986111111111109</v>
       </c>
-      <c r="C154" s="9" t="s">
+      <c r="C154" s="60" t="s">
         <v>307</v>
       </c>
-      <c r="D154" t="s">
+      <c r="D154" s="61" t="s">
         <v>324</v>
       </c>
-      <c r="E154" s="9">
+      <c r="E154" s="60">
         <v>1.6</v>
       </c>
-      <c r="F154" s="9">
-        <v>0.04</v>
-      </c>
-      <c r="G154" s="9">
-        <v>4</v>
-      </c>
-      <c r="H154" s="9">
-        <v>1</v>
-      </c>
-      <c r="I154" s="9">
-        <v>0</v>
-      </c>
-      <c r="J154" s="9">
-        <v>0.5</v>
-      </c>
-      <c r="L154" s="4" t="s">
+      <c r="F154" s="60">
+        <v>0.04</v>
+      </c>
+      <c r="G154" s="60">
+        <v>4</v>
+      </c>
+      <c r="H154" s="60">
+        <v>1</v>
+      </c>
+      <c r="I154" s="60">
+        <v>0</v>
+      </c>
+      <c r="J154" s="60">
+        <v>0.5</v>
+      </c>
+      <c r="K154" s="60">
+        <v>10</v>
+      </c>
+      <c r="M154" s="62" t="s">
         <v>315</v>
       </c>
     </row>
-    <row r="155" spans="1:12" ht="34" x14ac:dyDescent="0.2">
-      <c r="A155" s="5">
+    <row r="155" spans="1:13" s="61" customFormat="1" ht="34" x14ac:dyDescent="0.2">
+      <c r="A155" s="58">
         <v>44295</v>
       </c>
-      <c r="B155" s="3">
+      <c r="B155" s="59">
         <v>0.64444444444444449</v>
       </c>
-      <c r="C155" s="9" t="s">
+      <c r="C155" s="60" t="s">
         <v>308</v>
       </c>
-      <c r="D155" t="s">
+      <c r="D155" s="61" t="s">
         <v>323</v>
       </c>
-      <c r="E155" s="9">
+      <c r="E155" s="60">
         <v>1.6</v>
       </c>
-      <c r="F155" s="9">
-        <v>0.04</v>
-      </c>
-      <c r="G155" s="9">
-        <v>4</v>
-      </c>
-      <c r="H155" s="9">
-        <v>1</v>
-      </c>
-      <c r="I155" s="9">
-        <v>0</v>
-      </c>
-      <c r="J155" s="9">
-        <v>0.5</v>
-      </c>
-      <c r="L155" s="4" t="s">
+      <c r="F155" s="60">
+        <v>0.04</v>
+      </c>
+      <c r="G155" s="60">
+        <v>4</v>
+      </c>
+      <c r="H155" s="60">
+        <v>1</v>
+      </c>
+      <c r="I155" s="60">
+        <v>0</v>
+      </c>
+      <c r="J155" s="60">
+        <v>0.5</v>
+      </c>
+      <c r="K155" s="60">
+        <v>10</v>
+      </c>
+      <c r="M155" s="62" t="s">
         <v>316</v>
       </c>
     </row>
-    <row r="156" spans="1:12" ht="51" x14ac:dyDescent="0.2">
-      <c r="A156" s="5">
+    <row r="156" spans="1:13" s="61" customFormat="1" ht="51" x14ac:dyDescent="0.2">
+      <c r="A156" s="58">
         <v>44295</v>
       </c>
-      <c r="B156" s="3">
+      <c r="B156" s="59">
         <v>0.71111111111111114</v>
       </c>
-      <c r="C156" s="9" t="s">
+      <c r="C156" s="60" t="s">
         <v>262</v>
       </c>
-      <c r="D156" t="s">
+      <c r="D156" s="61" t="s">
         <v>322</v>
       </c>
-      <c r="E156" s="9">
+      <c r="E156" s="60">
         <v>1.6</v>
       </c>
-      <c r="F156" s="9">
-        <v>0.04</v>
-      </c>
-      <c r="G156" s="9">
-        <v>4</v>
-      </c>
-      <c r="H156" s="9">
-        <v>1</v>
-      </c>
-      <c r="I156" s="9">
-        <v>0</v>
-      </c>
-      <c r="J156" s="9">
-        <v>0.5</v>
-      </c>
-      <c r="L156" s="4" t="s">
+      <c r="F156" s="60">
+        <v>0.04</v>
+      </c>
+      <c r="G156" s="60">
+        <v>4</v>
+      </c>
+      <c r="H156" s="60">
+        <v>1</v>
+      </c>
+      <c r="I156" s="60">
+        <v>0</v>
+      </c>
+      <c r="J156" s="60">
+        <v>0.5</v>
+      </c>
+      <c r="K156" s="60">
+        <v>10</v>
+      </c>
+      <c r="M156" s="62" t="s">
         <v>317</v>
       </c>
     </row>
-    <row r="157" spans="1:12" ht="51" x14ac:dyDescent="0.2">
-      <c r="A157" s="5">
+    <row r="157" spans="1:13" s="61" customFormat="1" ht="51" x14ac:dyDescent="0.2">
+      <c r="A157" s="58">
         <v>44295</v>
       </c>
-      <c r="B157" s="3">
+      <c r="B157" s="59">
         <v>0.71944444444444444</v>
       </c>
-      <c r="C157" s="9" t="s">
+      <c r="C157" s="60" t="s">
         <v>261</v>
       </c>
-      <c r="D157" t="s">
+      <c r="D157" s="61" t="s">
         <v>321</v>
       </c>
-      <c r="E157" s="9">
+      <c r="E157" s="60">
         <v>1.6</v>
       </c>
-      <c r="F157" s="9">
-        <v>0.04</v>
-      </c>
-      <c r="G157" s="9">
-        <v>4</v>
-      </c>
-      <c r="H157" s="9">
-        <v>1</v>
-      </c>
-      <c r="I157" s="9">
-        <v>0</v>
-      </c>
-      <c r="J157" s="9">
-        <v>0.5</v>
-      </c>
-      <c r="L157" s="4" t="s">
+      <c r="F157" s="60">
+        <v>0.04</v>
+      </c>
+      <c r="G157" s="60">
+        <v>4</v>
+      </c>
+      <c r="H157" s="60">
+        <v>1</v>
+      </c>
+      <c r="I157" s="60">
+        <v>0</v>
+      </c>
+      <c r="J157" s="60">
+        <v>0.5</v>
+      </c>
+      <c r="K157" s="60">
+        <v>10</v>
+      </c>
+      <c r="M157" s="62" t="s">
         <v>318</v>
       </c>
     </row>
-    <row r="158" spans="1:12" ht="85" x14ac:dyDescent="0.2">
-      <c r="A158" s="5">
+    <row r="158" spans="1:13" s="61" customFormat="1" ht="85" x14ac:dyDescent="0.2">
+      <c r="A158" s="58">
         <v>44295</v>
       </c>
-      <c r="B158" s="3">
+      <c r="B158" s="59">
         <v>0.72638888888888886</v>
       </c>
-      <c r="C158" s="9" t="s">
+      <c r="C158" s="60" t="s">
         <v>262</v>
       </c>
-      <c r="D158" t="s">
+      <c r="D158" s="61" t="s">
         <v>320</v>
       </c>
-      <c r="E158" s="9">
+      <c r="E158" s="60">
         <v>1.6</v>
       </c>
-      <c r="F158" s="9">
-        <v>0.04</v>
-      </c>
-      <c r="G158" s="9">
-        <v>4</v>
-      </c>
-      <c r="H158" s="9">
-        <v>1</v>
-      </c>
-      <c r="I158" s="9">
-        <v>0</v>
-      </c>
-      <c r="J158" s="9">
-        <v>0.5</v>
-      </c>
-      <c r="L158" s="4" t="s">
+      <c r="F158" s="60">
+        <v>0.04</v>
+      </c>
+      <c r="G158" s="60">
+        <v>4</v>
+      </c>
+      <c r="H158" s="60">
+        <v>1</v>
+      </c>
+      <c r="I158" s="60">
+        <v>0</v>
+      </c>
+      <c r="J158" s="60">
+        <v>0.5</v>
+      </c>
+      <c r="K158" s="60">
+        <v>10</v>
+      </c>
+      <c r="M158" s="62" t="s">
         <v>319</v>
+      </c>
+    </row>
+    <row r="159" spans="1:13" ht="68" x14ac:dyDescent="0.2">
+      <c r="A159" s="5">
+        <v>44296</v>
+      </c>
+      <c r="B159" s="3">
+        <v>0.60902777777777783</v>
+      </c>
+      <c r="C159" s="35" t="s">
+        <v>307</v>
+      </c>
+      <c r="D159" t="s">
+        <v>358</v>
+      </c>
+      <c r="E159" s="9">
+        <v>1.6</v>
+      </c>
+      <c r="F159" s="9">
+        <v>0.04</v>
+      </c>
+      <c r="G159" s="9">
+        <v>4</v>
+      </c>
+      <c r="H159" s="9">
+        <v>1</v>
+      </c>
+      <c r="I159" s="9">
+        <v>0</v>
+      </c>
+      <c r="J159" s="9">
+        <v>0.5</v>
+      </c>
+      <c r="K159" s="9">
+        <v>0</v>
+      </c>
+      <c r="M159" s="37" t="s">
+        <v>354</v>
+      </c>
+    </row>
+    <row r="160" spans="1:13" ht="34" x14ac:dyDescent="0.2">
+      <c r="A160" s="5">
+        <v>44296</v>
+      </c>
+      <c r="B160" s="3">
+        <v>0.62361111111111112</v>
+      </c>
+      <c r="C160" s="35" t="s">
+        <v>308</v>
+      </c>
+      <c r="D160" t="s">
+        <v>359</v>
+      </c>
+      <c r="E160" s="9">
+        <v>1.6</v>
+      </c>
+      <c r="F160" s="9">
+        <v>0.04</v>
+      </c>
+      <c r="G160" s="9">
+        <v>4</v>
+      </c>
+      <c r="H160" s="9">
+        <v>1</v>
+      </c>
+      <c r="I160" s="9">
+        <v>0</v>
+      </c>
+      <c r="J160" s="9">
+        <v>0.5</v>
+      </c>
+      <c r="K160" s="9">
+        <v>0</v>
+      </c>
+      <c r="M160" s="37" t="s">
+        <v>355</v>
+      </c>
+    </row>
+    <row r="161" spans="1:13" ht="68" x14ac:dyDescent="0.2">
+      <c r="A161" s="5">
+        <v>44296</v>
+      </c>
+      <c r="B161" s="3">
+        <v>0.6381944444444444</v>
+      </c>
+      <c r="C161" s="35" t="s">
+        <v>307</v>
+      </c>
+      <c r="D161" t="s">
+        <v>360</v>
+      </c>
+      <c r="E161" s="9">
+        <v>1.6</v>
+      </c>
+      <c r="F161" s="9">
+        <v>0.04</v>
+      </c>
+      <c r="G161" s="9">
+        <v>4</v>
+      </c>
+      <c r="H161" s="9">
+        <v>1</v>
+      </c>
+      <c r="I161" s="9">
+        <v>0</v>
+      </c>
+      <c r="J161" s="9">
+        <v>0.5</v>
+      </c>
+      <c r="K161" s="9">
+        <v>0</v>
+      </c>
+      <c r="M161" s="37" t="s">
+        <v>354</v>
+      </c>
+    </row>
+    <row r="162" spans="1:13" ht="34" x14ac:dyDescent="0.2">
+      <c r="A162" s="5">
+        <v>44296</v>
+      </c>
+      <c r="B162" s="3">
+        <v>0.65277777777777779</v>
+      </c>
+      <c r="C162" s="35" t="s">
+        <v>308</v>
+      </c>
+      <c r="D162" t="s">
+        <v>361</v>
+      </c>
+      <c r="E162" s="9">
+        <v>1.6</v>
+      </c>
+      <c r="F162" s="9">
+        <v>0.04</v>
+      </c>
+      <c r="G162" s="9">
+        <v>4</v>
+      </c>
+      <c r="H162" s="9">
+        <v>1</v>
+      </c>
+      <c r="I162" s="9">
+        <v>0</v>
+      </c>
+      <c r="J162" s="9">
+        <v>0.5</v>
+      </c>
+      <c r="K162" s="9">
+        <v>0</v>
+      </c>
+      <c r="M162" s="37" t="s">
+        <v>355</v>
+      </c>
+    </row>
+    <row r="163" spans="1:13" ht="85" x14ac:dyDescent="0.2">
+      <c r="A163" s="5">
+        <v>44296</v>
+      </c>
+      <c r="B163" s="3">
+        <v>0.66805555555555562</v>
+      </c>
+      <c r="C163" s="35" t="s">
+        <v>307</v>
+      </c>
+      <c r="D163" t="s">
+        <v>362</v>
+      </c>
+      <c r="E163" s="9">
+        <v>1.6</v>
+      </c>
+      <c r="F163" s="9">
+        <v>0.04</v>
+      </c>
+      <c r="G163" s="9">
+        <v>4</v>
+      </c>
+      <c r="H163" s="9">
+        <v>1</v>
+      </c>
+      <c r="I163" s="9">
+        <v>0</v>
+      </c>
+      <c r="J163" s="9">
+        <v>0.5</v>
+      </c>
+      <c r="K163" s="9">
+        <v>0</v>
+      </c>
+      <c r="M163" s="37" t="s">
+        <v>356</v>
+      </c>
+    </row>
+    <row r="164" spans="1:13" ht="34" x14ac:dyDescent="0.2">
+      <c r="A164" s="5">
+        <v>44296</v>
+      </c>
+      <c r="B164" s="3">
+        <v>0.68263888888888891</v>
+      </c>
+      <c r="C164" s="35" t="s">
+        <v>308</v>
+      </c>
+      <c r="D164" t="s">
+        <v>363</v>
+      </c>
+      <c r="E164" s="9">
+        <v>1.6</v>
+      </c>
+      <c r="F164" s="9">
+        <v>0.04</v>
+      </c>
+      <c r="G164" s="9">
+        <v>4</v>
+      </c>
+      <c r="H164" s="9">
+        <v>1</v>
+      </c>
+      <c r="I164" s="9">
+        <v>0</v>
+      </c>
+      <c r="J164" s="9">
+        <v>0.5</v>
+      </c>
+      <c r="K164" s="9">
+        <v>0</v>
+      </c>
+      <c r="M164" s="37" t="s">
+        <v>355</v>
+      </c>
+    </row>
+    <row r="165" spans="1:13" ht="17" x14ac:dyDescent="0.2">
+      <c r="A165" s="5">
+        <v>44296</v>
+      </c>
+      <c r="B165" s="3">
+        <v>0.71875</v>
+      </c>
+      <c r="C165" s="35" t="s">
+        <v>284</v>
+      </c>
+      <c r="D165" t="s">
+        <v>364</v>
+      </c>
+      <c r="E165" s="9">
+        <v>0.4</v>
+      </c>
+      <c r="F165" s="9">
+        <v>0.04</v>
+      </c>
+      <c r="G165" s="9">
+        <v>4</v>
+      </c>
+      <c r="H165" s="9">
+        <v>1</v>
+      </c>
+      <c r="I165" s="9">
+        <v>0</v>
+      </c>
+      <c r="J165" s="9">
+        <v>0.5</v>
+      </c>
+      <c r="M165" s="37" t="s">
+        <v>357</v>
       </c>
     </row>
   </sheetData>

</xml_diff>